<commit_message>
added nist pretty latex output
</commit_message>
<xml_diff>
--- a/python_src/nist_confusion/confusion_matrix_0.0.xlsx
+++ b/python_src/nist_confusion/confusion_matrix_0.0.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,188 +438,197 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>species</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>tp</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>fp</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>fn</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>tn</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>sens</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>spec</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>prec</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>acc</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>f1</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Threshold</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>ACHROMOBACTER_XYLOSOXIDANS</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>3</v>
       </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
       <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="n">
         <v>0.75</v>
       </c>
-      <c r="G2" t="n">
-        <v>1</v>
-      </c>
       <c r="H2" t="n">
         <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J2" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K2" t="n">
         <v>0.8571428571428571</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>ACINETOBACTER_BAUMANNII</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>3</v>
       </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
         <v>1</v>
       </c>
       <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="n">
         <v>0.75</v>
       </c>
-      <c r="G3" t="n">
-        <v>1</v>
-      </c>
       <c r="H3" t="n">
         <v>1</v>
       </c>
       <c r="I3" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J3" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K3" t="n">
         <v>0.8571428571428571</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>AEROMONAS_HYDROPHILA</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>4</v>
-      </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="n">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J4" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K4" t="n">
         <v>0.888888888888889</v>
       </c>
-      <c r="K4" t="n">
+      <c r="L4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>ENTEROCOCCUS_FAECALIS</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>4</v>
-      </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
         <v>1</v>
@@ -637,95 +646,104 @@
         <v>1</v>
       </c>
       <c r="K5" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>ESCHERICHIA_COLI</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>4</v>
-      </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
         <v>0.8</v>
       </c>
       <c r="J6" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K6" t="n">
         <v>0.888888888888889</v>
       </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>KLEBSIELLA_PNEUMONIAE</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="C7" t="n">
         <v>3</v>
       </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
         <v>1</v>
       </c>
       <c r="F7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" t="n">
         <v>0.75</v>
       </c>
-      <c r="G7" t="n">
-        <v>1</v>
-      </c>
       <c r="H7" t="n">
         <v>1</v>
       </c>
       <c r="I7" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J7" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K7" t="n">
         <v>0.8571428571428571</v>
       </c>
-      <c r="K7" t="n">
+      <c r="L7" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>LEGIONELLA_PNEUMOPHILA</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="C8" t="n">
         <v>5</v>
       </c>
-      <c r="C8" t="n">
-        <v>0</v>
-      </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
@@ -733,12 +751,12 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="n">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" t="inlineStr"/>
       <c r="I8" t="n">
         <v>1</v>
       </c>
@@ -746,319 +764,349 @@
         <v>1</v>
       </c>
       <c r="K8" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>LISTERIA_MONOCYTOGENES</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="C9" t="n">
         <v>3</v>
       </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
         <v>1</v>
       </c>
       <c r="F9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" t="n">
         <v>0.75</v>
       </c>
-      <c r="G9" t="n">
-        <v>1</v>
-      </c>
       <c r="H9" t="n">
         <v>1</v>
       </c>
       <c r="I9" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J9" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K9" t="n">
         <v>0.8571428571428571</v>
       </c>
-      <c r="K9" t="n">
+      <c r="L9" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
         <is>
           <t>NEISSERIA_MENINGITIDIS</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="C10" t="n">
         <v>3</v>
       </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
         <v>1</v>
       </c>
       <c r="F10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" t="n">
         <v>0.75</v>
       </c>
-      <c r="G10" t="n">
-        <v>1</v>
-      </c>
       <c r="H10" t="n">
         <v>1</v>
       </c>
       <c r="I10" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J10" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K10" t="n">
         <v>0.8571428571428571</v>
       </c>
-      <c r="K10" t="n">
+      <c r="L10" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="inlineStr">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>SALMONELLA_ENTERICA</t>
         </is>
       </c>
-      <c r="B11" t="n">
+      <c r="C11" t="n">
         <v>3</v>
       </c>
-      <c r="C11" t="n">
-        <v>0</v>
-      </c>
       <c r="D11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" t="n">
         <v>1</v>
       </c>
       <c r="F11" t="n">
+        <v>1</v>
+      </c>
+      <c r="G11" t="n">
         <v>0.75</v>
       </c>
-      <c r="G11" t="n">
-        <v>1</v>
-      </c>
       <c r="H11" t="n">
         <v>1</v>
       </c>
       <c r="I11" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J11" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K11" t="n">
         <v>0.8571428571428571</v>
       </c>
-      <c r="K11" t="n">
+      <c r="L11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>SHIGELLA_SONNEI</t>
         </is>
       </c>
-      <c r="B12" t="n">
-        <v>0</v>
-      </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" t="n">
-        <v>1</v>
-      </c>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="n">
         <v>0.2</v>
       </c>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="n">
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="inlineStr">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
         <is>
           <t>STAPHYLOCOCCUS_AUREUS</t>
         </is>
       </c>
-      <c r="B13" t="n">
+      <c r="C13" t="n">
         <v>3</v>
       </c>
-      <c r="C13" t="n">
-        <v>0</v>
-      </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" t="n">
         <v>1</v>
       </c>
       <c r="F13" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" t="n">
         <v>0.75</v>
       </c>
-      <c r="G13" t="n">
-        <v>1</v>
-      </c>
       <c r="H13" t="n">
         <v>1</v>
       </c>
       <c r="I13" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J13" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K13" t="n">
         <v>0.8571428571428571</v>
       </c>
-      <c r="K13" t="n">
+      <c r="L13" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="inlineStr">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
         <is>
           <t>STREPTOCOCCUS_PYOGENES</t>
         </is>
       </c>
-      <c r="B14" t="n">
+      <c r="C14" t="n">
         <v>3</v>
       </c>
-      <c r="C14" t="n">
-        <v>0</v>
-      </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" t="n">
         <v>1</v>
       </c>
       <c r="F14" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" t="n">
         <v>0.75</v>
       </c>
-      <c r="G14" t="n">
-        <v>1</v>
-      </c>
       <c r="H14" t="n">
         <v>1</v>
       </c>
       <c r="I14" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J14" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K14" t="n">
         <v>0.8571428571428571</v>
       </c>
-      <c r="K14" t="n">
+      <c r="L14" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="inlineStr">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
         <is>
           <t>VIBRIO_FURNISSII</t>
         </is>
       </c>
-      <c r="B15" t="n">
+      <c r="C15" t="n">
         <v>3</v>
       </c>
-      <c r="C15" t="n">
-        <v>0</v>
-      </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" t="n">
         <v>1</v>
       </c>
       <c r="F15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" t="n">
         <v>0.75</v>
       </c>
-      <c r="G15" t="n">
-        <v>1</v>
-      </c>
       <c r="H15" t="n">
         <v>1</v>
       </c>
       <c r="I15" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J15" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K15" t="n">
         <v>0.8571428571428571</v>
       </c>
-      <c r="K15" t="n">
+      <c r="L15" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="inlineStr">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
         <is>
           <t>Harmonic Mean</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
-      <c r="F16" t="n">
-        <v>0</v>
-      </c>
+      <c r="F16" t="inlineStr"/>
       <c r="G16" t="n">
         <v>0</v>
       </c>
       <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
         <v>0.9811320754716981</v>
       </c>
-      <c r="I16" t="n">
+      <c r="J16" t="n">
         <v>0.6746987951807228</v>
       </c>
-      <c r="J16" t="n">
+      <c r="K16" t="n">
         <v>0.8813559322033899</v>
       </c>
-      <c r="K16" t="n">
+      <c r="L16" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="inlineStr">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
         <is>
           <t>Mean</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
-      <c r="F17" t="n">
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="n">
         <v>0.7033333333333334</v>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
         <v>0.8461538461538461</v>
       </c>
-      <c r="H17" t="n">
+      <c r="I17" t="n">
         <v>0.9843665768194071</v>
       </c>
-      <c r="I17" t="n">
+      <c r="J17" t="n">
         <v>0.7783132530120482</v>
       </c>
-      <c r="J17" t="n">
+      <c r="K17" t="n">
         <v>0.8838156731619202</v>
       </c>
-      <c r="K17" t="n">
+      <c r="L17" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1073,7 +1121,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1082,148 +1130,154 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>species</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>tp</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>fp</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>fn</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>tn</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>sens</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>spec</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>prec</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>acc</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>f1</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Threshold</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>ACHROMOBACTER_XYLOSOXIDANS</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>3</v>
       </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
       <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="n">
         <v>0.75</v>
       </c>
-      <c r="G2" t="n">
-        <v>1</v>
-      </c>
       <c r="H2" t="n">
         <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J2" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K2" t="n">
         <v>0.8571428571428571</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>ACINETOBACTER_BAUMANNII</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>3</v>
       </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
         <v>1</v>
       </c>
       <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="n">
         <v>0.75</v>
       </c>
-      <c r="G3" t="n">
-        <v>1</v>
-      </c>
       <c r="H3" t="n">
         <v>1</v>
       </c>
       <c r="I3" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J3" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K3" t="n">
         <v>0.8571428571428571</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>AEROMONAS_HYDROPHILA</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="C4" t="n">
         <v>5</v>
       </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
@@ -1231,12 +1285,12 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="n">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="n">
         <v>1</v>
       </c>
@@ -1244,26 +1298,29 @@
         <v>1</v>
       </c>
       <c r="K4" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>ENTEROCOCCUS_FAECALIS</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>4</v>
-      </c>
       <c r="C5" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D5" t="n">
         <v>0</v>
       </c>
       <c r="E5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F5" t="n">
         <v>1</v>
@@ -1281,95 +1338,104 @@
         <v>1</v>
       </c>
       <c r="K5" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>ESCHERICHIA_COLI</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>4</v>
-      </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
         <v>0.8</v>
       </c>
       <c r="J6" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K6" t="n">
         <v>0.888888888888889</v>
       </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>KLEBSIELLA_PNEUMONIAE</t>
         </is>
       </c>
-      <c r="B7" t="n">
+      <c r="C7" t="n">
         <v>3</v>
       </c>
-      <c r="C7" t="n">
-        <v>0</v>
-      </c>
       <c r="D7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
         <v>1</v>
       </c>
       <c r="F7" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" t="n">
         <v>0.75</v>
       </c>
-      <c r="G7" t="n">
-        <v>1</v>
-      </c>
       <c r="H7" t="n">
         <v>1</v>
       </c>
       <c r="I7" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J7" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K7" t="n">
         <v>0.8571428571428571</v>
       </c>
-      <c r="K7" t="n">
+      <c r="L7" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>LEGIONELLA_PNEUMOPHILA</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="C8" t="n">
         <v>5</v>
       </c>
-      <c r="C8" t="n">
-        <v>0</v>
-      </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
@@ -1377,12 +1443,12 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="n">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" t="inlineStr"/>
       <c r="I8" t="n">
         <v>1</v>
       </c>
@@ -1390,244 +1456,265 @@
         <v>1</v>
       </c>
       <c r="K8" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>LISTERIA_MONOCYTOGENES</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="C9" t="n">
         <v>3</v>
       </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
         <v>1</v>
       </c>
       <c r="F9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" t="n">
         <v>0.75</v>
       </c>
-      <c r="G9" t="n">
-        <v>1</v>
-      </c>
       <c r="H9" t="n">
         <v>1</v>
       </c>
       <c r="I9" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J9" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K9" t="n">
         <v>0.8571428571428571</v>
       </c>
-      <c r="K9" t="n">
+      <c r="L9" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
         <is>
           <t>NEISSERIA_MENINGITIDIS</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="C10" t="n">
         <v>3</v>
       </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
         <v>1</v>
       </c>
       <c r="F10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" t="n">
         <v>0.75</v>
       </c>
-      <c r="G10" t="n">
-        <v>1</v>
-      </c>
       <c r="H10" t="n">
         <v>1</v>
       </c>
       <c r="I10" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J10" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K10" t="n">
         <v>0.8571428571428571</v>
       </c>
-      <c r="K10" t="n">
+      <c r="L10" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="inlineStr">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>SALMONELLA_ENTERICA</t>
         </is>
       </c>
-      <c r="B11" t="n">
+      <c r="C11" t="n">
         <v>3</v>
       </c>
-      <c r="C11" t="n">
-        <v>1</v>
-      </c>
       <c r="D11" t="n">
         <v>1</v>
       </c>
       <c r="E11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F11" t="n">
+        <v>0</v>
+      </c>
+      <c r="G11" t="n">
         <v>0.75</v>
       </c>
-      <c r="G11" t="n">
-        <v>0</v>
-      </c>
       <c r="H11" t="n">
+        <v>0</v>
+      </c>
+      <c r="I11" t="n">
         <v>0.75</v>
       </c>
-      <c r="I11" t="n">
+      <c r="J11" t="n">
         <v>0.6</v>
       </c>
-      <c r="J11" t="n">
+      <c r="K11" t="n">
         <v>0.75</v>
       </c>
-      <c r="K11" t="n">
+      <c r="L11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>SHIGELLA_SONNEI</t>
         </is>
       </c>
-      <c r="B12" t="n">
-        <v>0</v>
-      </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" t="n">
-        <v>1</v>
-      </c>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="n">
         <v>0.2</v>
       </c>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="n">
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="inlineStr">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
         <is>
           <t>STAPHYLOCOCCUS_AUREUS</t>
         </is>
       </c>
-      <c r="B13" t="n">
+      <c r="C13" t="n">
         <v>3</v>
       </c>
-      <c r="C13" t="n">
-        <v>0</v>
-      </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" t="n">
         <v>1</v>
       </c>
       <c r="F13" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" t="n">
         <v>0.75</v>
       </c>
-      <c r="G13" t="n">
-        <v>1</v>
-      </c>
       <c r="H13" t="n">
         <v>1</v>
       </c>
       <c r="I13" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J13" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K13" t="n">
         <v>0.8571428571428571</v>
       </c>
-      <c r="K13" t="n">
+      <c r="L13" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="inlineStr">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
         <is>
           <t>STREPTOCOCCUS_PYOGENES</t>
         </is>
       </c>
-      <c r="B14" t="n">
+      <c r="C14" t="n">
         <v>3</v>
       </c>
-      <c r="C14" t="n">
-        <v>0</v>
-      </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" t="n">
         <v>1</v>
       </c>
       <c r="F14" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" t="n">
         <v>0.75</v>
       </c>
-      <c r="G14" t="n">
-        <v>1</v>
-      </c>
       <c r="H14" t="n">
         <v>1</v>
       </c>
       <c r="I14" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J14" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K14" t="n">
         <v>0.8571428571428571</v>
       </c>
-      <c r="K14" t="n">
+      <c r="L14" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="inlineStr">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
         <is>
           <t>VIBRIO_FURNISSII</t>
         </is>
       </c>
-      <c r="B15" t="n">
-        <v>4</v>
-      </c>
       <c r="C15" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D15" t="n">
         <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F15" t="n">
         <v>1</v>
@@ -1645,64 +1732,73 @@
         <v>1</v>
       </c>
       <c r="K15" t="n">
+        <v>1</v>
+      </c>
+      <c r="L15" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="inlineStr">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
         <is>
           <t>Harmonic Mean</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
-      <c r="F16" t="n">
-        <v>0</v>
-      </c>
+      <c r="F16" t="inlineStr"/>
       <c r="G16" t="n">
         <v>0</v>
       </c>
       <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
         <v>0.9570552147239263</v>
       </c>
-      <c r="I16" t="n">
+      <c r="J16" t="n">
         <v>0.6774193548387097</v>
       </c>
-      <c r="J16" t="n">
+      <c r="K16" t="n">
         <v>0.8888888888888888</v>
       </c>
-      <c r="K16" t="n">
+      <c r="L16" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="inlineStr">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
         <is>
           <t>Mean</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
-      <c r="F17" t="n">
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="n">
         <v>0.7333333333333333</v>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
         <v>0.7692307692307693</v>
       </c>
-      <c r="H17" t="n">
+      <c r="I17" t="n">
         <v>0.9647896581945662</v>
       </c>
-      <c r="I17" t="n">
+      <c r="J17" t="n">
         <v>0.7918279569892474</v>
       </c>
-      <c r="J17" t="n">
+      <c r="K17" t="n">
         <v>0.89484126984127</v>
       </c>
-      <c r="K17" t="n">
+      <c r="L17" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1717,7 +1813,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1726,262 +1822,277 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>species</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>tp</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>fp</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>fn</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>tn</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>sens</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>spec</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>prec</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>acc</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>f1</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Threshold</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>ACHROMOBACTER_XYLOSOXIDANS</t>
         </is>
       </c>
-      <c r="B2" t="n">
+      <c r="C2" t="n">
         <v>3</v>
       </c>
-      <c r="C2" t="n">
-        <v>0</v>
-      </c>
       <c r="D2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E2" t="n">
         <v>1</v>
       </c>
       <c r="F2" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" t="n">
         <v>0.75</v>
       </c>
-      <c r="G2" t="n">
-        <v>1</v>
-      </c>
       <c r="H2" t="n">
         <v>1</v>
       </c>
       <c r="I2" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J2" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K2" t="n">
         <v>0.8571428571428571</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>ACINETOBACTER_BAUMANNII</t>
         </is>
       </c>
-      <c r="B3" t="n">
+      <c r="C3" t="n">
         <v>3</v>
       </c>
-      <c r="C3" t="n">
-        <v>0</v>
-      </c>
       <c r="D3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3" t="n">
         <v>1</v>
       </c>
       <c r="F3" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" t="n">
         <v>0.75</v>
       </c>
-      <c r="G3" t="n">
-        <v>1</v>
-      </c>
       <c r="H3" t="n">
         <v>1</v>
       </c>
       <c r="I3" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J3" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K3" t="n">
         <v>0.8571428571428571</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>AEROMONAS_HYDROPHILA</t>
         </is>
       </c>
-      <c r="B4" t="n">
-        <v>4</v>
-      </c>
       <c r="C4" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F4" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="n">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J4" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K4" t="n">
         <v>0.888888888888889</v>
       </c>
-      <c r="K4" t="n">
+      <c r="L4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>ENTEROCOCCUS_FAECALIS</t>
         </is>
       </c>
-      <c r="B5" t="n">
+      <c r="C5" t="n">
         <v>3</v>
       </c>
-      <c r="C5" t="n">
-        <v>0</v>
-      </c>
       <c r="D5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5" t="n">
         <v>1</v>
       </c>
       <c r="F5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" t="n">
         <v>0.75</v>
       </c>
-      <c r="G5" t="n">
-        <v>1</v>
-      </c>
       <c r="H5" t="n">
         <v>1</v>
       </c>
       <c r="I5" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J5" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K5" t="n">
         <v>0.8571428571428571</v>
       </c>
-      <c r="K5" t="n">
+      <c r="L5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>ESCHERICHIA_COLI</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>4</v>
-      </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
         <v>0.8</v>
       </c>
       <c r="J6" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K6" t="n">
         <v>0.888888888888889</v>
       </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>KLEBSIELLA_PNEUMONIAE</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>4</v>
-      </c>
       <c r="C7" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D7" t="n">
         <v>0</v>
       </c>
       <c r="E7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F7" t="n">
         <v>1</v>
@@ -1999,21 +2110,24 @@
         <v>1</v>
       </c>
       <c r="K7" t="n">
+        <v>1</v>
+      </c>
+      <c r="L7" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>LEGIONELLA_PNEUMOPHILA</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="C8" t="n">
         <v>5</v>
       </c>
-      <c r="C8" t="n">
-        <v>0</v>
-      </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
@@ -2021,12 +2135,12 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="n">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" t="inlineStr"/>
       <c r="I8" t="n">
         <v>1</v>
       </c>
@@ -2034,137 +2148,149 @@
         <v>1</v>
       </c>
       <c r="K8" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>LISTERIA_MONOCYTOGENES</t>
         </is>
       </c>
-      <c r="B9" t="n">
+      <c r="C9" t="n">
         <v>3</v>
       </c>
-      <c r="C9" t="n">
-        <v>0</v>
-      </c>
       <c r="D9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E9" t="n">
         <v>1</v>
       </c>
       <c r="F9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G9" t="n">
         <v>0.75</v>
       </c>
-      <c r="G9" t="n">
-        <v>1</v>
-      </c>
       <c r="H9" t="n">
         <v>1</v>
       </c>
       <c r="I9" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J9" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K9" t="n">
         <v>0.8571428571428571</v>
       </c>
-      <c r="K9" t="n">
+      <c r="L9" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
         <is>
           <t>NEISSERIA_MENINGITIDIS</t>
         </is>
       </c>
-      <c r="B10" t="n">
+      <c r="C10" t="n">
         <v>3</v>
       </c>
-      <c r="C10" t="n">
-        <v>0</v>
-      </c>
       <c r="D10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E10" t="n">
         <v>1</v>
       </c>
       <c r="F10" t="n">
+        <v>1</v>
+      </c>
+      <c r="G10" t="n">
         <v>0.75</v>
       </c>
-      <c r="G10" t="n">
-        <v>1</v>
-      </c>
       <c r="H10" t="n">
         <v>1</v>
       </c>
       <c r="I10" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J10" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K10" t="n">
         <v>0.8571428571428571</v>
       </c>
-      <c r="K10" t="n">
+      <c r="L10" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="inlineStr">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>SALMONELLA_ENTERICA</t>
         </is>
       </c>
-      <c r="B11" t="n">
-        <v>4</v>
-      </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="I11" t="n">
         <v>0.8</v>
       </c>
       <c r="J11" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K11" t="n">
         <v>0.888888888888889</v>
       </c>
-      <c r="K11" t="n">
+      <c r="L11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>SHIGELLA_SONNEI</t>
         </is>
       </c>
-      <c r="B12" t="n">
-        <v>4</v>
-      </c>
       <c r="C12" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D12" t="n">
         <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F12" t="n">
         <v>1</v>
@@ -2182,175 +2308,193 @@
         <v>1</v>
       </c>
       <c r="K12" t="n">
+        <v>1</v>
+      </c>
+      <c r="L12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="inlineStr">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
         <is>
           <t>STAPHYLOCOCCUS_AUREUS</t>
         </is>
       </c>
-      <c r="B13" t="n">
+      <c r="C13" t="n">
         <v>3</v>
       </c>
-      <c r="C13" t="n">
-        <v>0</v>
-      </c>
       <c r="D13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E13" t="n">
         <v>1</v>
       </c>
       <c r="F13" t="n">
+        <v>1</v>
+      </c>
+      <c r="G13" t="n">
         <v>0.75</v>
       </c>
-      <c r="G13" t="n">
-        <v>1</v>
-      </c>
       <c r="H13" t="n">
         <v>1</v>
       </c>
       <c r="I13" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J13" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K13" t="n">
         <v>0.8571428571428571</v>
       </c>
-      <c r="K13" t="n">
+      <c r="L13" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="inlineStr">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
         <is>
           <t>STREPTOCOCCUS_PYOGENES</t>
         </is>
       </c>
-      <c r="B14" t="n">
+      <c r="C14" t="n">
         <v>3</v>
       </c>
-      <c r="C14" t="n">
-        <v>0</v>
-      </c>
       <c r="D14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" t="n">
         <v>1</v>
       </c>
       <c r="F14" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" t="n">
         <v>0.75</v>
       </c>
-      <c r="G14" t="n">
-        <v>1</v>
-      </c>
       <c r="H14" t="n">
         <v>1</v>
       </c>
       <c r="I14" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J14" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K14" t="n">
         <v>0.8571428571428571</v>
       </c>
-      <c r="K14" t="n">
+      <c r="L14" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="inlineStr">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
         <is>
           <t>VIBRIO_FURNISSII</t>
         </is>
       </c>
-      <c r="B15" t="n">
+      <c r="C15" t="n">
         <v>3</v>
       </c>
-      <c r="C15" t="n">
-        <v>0</v>
-      </c>
       <c r="D15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" t="n">
         <v>1</v>
       </c>
       <c r="F15" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" t="n">
         <v>0.75</v>
       </c>
-      <c r="G15" t="n">
-        <v>1</v>
-      </c>
       <c r="H15" t="n">
         <v>1</v>
       </c>
       <c r="I15" t="n">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="J15" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K15" t="n">
         <v>0.8571428571428571</v>
       </c>
-      <c r="K15" t="n">
+      <c r="L15" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="inlineStr">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
         <is>
           <t>Harmonic Mean</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
-      <c r="F16" t="n">
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="n">
         <v>0.8275862068965517</v>
       </c>
-      <c r="G16" t="n">
-        <v>0</v>
-      </c>
       <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
         <v>0.9655172413793104</v>
       </c>
-      <c r="I16" t="n">
+      <c r="J16" t="n">
         <v>0.835820895522388</v>
       </c>
-      <c r="J16" t="n">
+      <c r="K16" t="n">
         <v>0.8912466843501327</v>
       </c>
-      <c r="K16" t="n">
+      <c r="L16" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="inlineStr">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
         <is>
           <t>Mean</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
-      <c r="F17" t="n">
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="n">
         <v>0.8418390804597702</v>
       </c>
-      <c r="G17" t="n">
+      <c r="H17" t="n">
         <v>0.7692307692307693</v>
       </c>
-      <c r="H17" t="n">
+      <c r="I17" t="n">
         <v>0.9710344827586207</v>
       </c>
-      <c r="I17" t="n">
+      <c r="J17" t="n">
         <v>0.8423880597014928</v>
       </c>
-      <c r="J17" t="n">
+      <c r="K17" t="n">
         <v>0.8943370805439772</v>
       </c>
-      <c r="K17" t="n">
+      <c r="L17" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2365,7 +2509,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2374,148 +2518,154 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>species</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>tp</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>fp</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>fn</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>tn</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>sens</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>spec</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>prec</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>acc</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>f1</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Threshold</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>ACHROMOBACTER_XYLOSOXIDANS</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>4</v>
-      </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
         <v>0.8</v>
       </c>
       <c r="J2" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K2" t="n">
         <v>0.888888888888889</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>ACINETOBACTER_BAUMANNII</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>4</v>
-      </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
         <v>0.8</v>
       </c>
       <c r="J3" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K3" t="n">
         <v>0.888888888888889</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>AEROMONAS_HYDROPHILA</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="C4" t="n">
         <v>5</v>
       </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
@@ -2523,12 +2673,12 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="n">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="n">
         <v>1</v>
       </c>
@@ -2536,132 +2686,144 @@
         <v>1</v>
       </c>
       <c r="K4" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>ENTEROCOCCUS_FAECALIS</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>4</v>
-      </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
         <v>0.8</v>
       </c>
       <c r="J5" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K5" t="n">
         <v>0.888888888888889</v>
       </c>
-      <c r="K5" t="n">
+      <c r="L5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>ESCHERICHIA_COLI</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>4</v>
-      </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
         <v>0.8</v>
       </c>
       <c r="J6" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K6" t="n">
         <v>0.888888888888889</v>
       </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>KLEBSIELLA_PNEUMONIAE</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>4</v>
-      </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
         <v>0.8</v>
       </c>
       <c r="J7" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K7" t="n">
         <v>0.888888888888889</v>
       </c>
-      <c r="K7" t="n">
+      <c r="L7" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>LEGIONELLA_PNEUMOPHILA</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="C8" t="n">
         <v>5</v>
       </c>
-      <c r="C8" t="n">
-        <v>0</v>
-      </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
@@ -2669,12 +2831,12 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="n">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" t="inlineStr"/>
       <c r="I8" t="n">
         <v>1</v>
       </c>
@@ -2682,323 +2844,353 @@
         <v>1</v>
       </c>
       <c r="K8" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>LISTERIA_MONOCYTOGENES</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>4</v>
-      </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="I9" t="n">
         <v>0.8</v>
       </c>
       <c r="J9" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K9" t="n">
         <v>0.888888888888889</v>
       </c>
-      <c r="K9" t="n">
+      <c r="L9" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
         <is>
           <t>NEISSERIA_MENINGITIDIS</t>
         </is>
       </c>
-      <c r="B10" t="n">
-        <v>4</v>
-      </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="I10" t="n">
         <v>0.8</v>
       </c>
       <c r="J10" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K10" t="n">
         <v>0.888888888888889</v>
       </c>
-      <c r="K10" t="n">
+      <c r="L10" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="inlineStr">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>SALMONELLA_ENTERICA</t>
         </is>
       </c>
-      <c r="B11" t="n">
-        <v>4</v>
-      </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="I11" t="n">
         <v>0.8</v>
       </c>
       <c r="J11" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K11" t="n">
         <v>0.888888888888889</v>
       </c>
-      <c r="K11" t="n">
+      <c r="L11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>SHIGELLA_SONNEI</t>
         </is>
       </c>
-      <c r="B12" t="n">
-        <v>4</v>
-      </c>
       <c r="C12" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E12" t="n">
         <v>0</v>
       </c>
       <c r="F12" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H12" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="I12" t="n">
         <v>0.8</v>
       </c>
       <c r="J12" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K12" t="n">
         <v>0.888888888888889</v>
       </c>
-      <c r="K12" t="n">
+      <c r="L12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="inlineStr">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
         <is>
           <t>STAPHYLOCOCCUS_AUREUS</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v>4</v>
-      </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="I13" t="n">
         <v>0.8</v>
       </c>
       <c r="J13" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K13" t="n">
         <v>0.888888888888889</v>
       </c>
-      <c r="K13" t="n">
+      <c r="L13" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="inlineStr">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
         <is>
           <t>STREPTOCOCCUS_PYOGENES</t>
         </is>
       </c>
-      <c r="B14" t="n">
-        <v>4</v>
-      </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="I14" t="n">
         <v>0.8</v>
       </c>
       <c r="J14" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K14" t="n">
         <v>0.888888888888889</v>
       </c>
-      <c r="K14" t="n">
+      <c r="L14" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="inlineStr">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
         <is>
           <t>VIBRIO_FURNISSII</t>
         </is>
       </c>
-      <c r="B15" t="n">
-        <v>4</v>
-      </c>
       <c r="C15" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" t="n">
         <v>0</v>
       </c>
       <c r="F15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="I15" t="n">
         <v>0.8</v>
       </c>
       <c r="J15" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K15" t="n">
         <v>0.888888888888889</v>
       </c>
-      <c r="K15" t="n">
+      <c r="L15" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="inlineStr">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
         <is>
           <t>Harmonic Mean</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
-      <c r="F16" t="n">
-        <v>1</v>
-      </c>
+      <c r="F16" t="inlineStr"/>
       <c r="G16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H16" t="n">
-        <v>0.8235294117647058</v>
+        <v>0</v>
       </c>
       <c r="I16" t="n">
         <v>0.8235294117647058</v>
       </c>
       <c r="J16" t="n">
+        <v>0.8235294117647058</v>
+      </c>
+      <c r="K16" t="n">
         <v>0.9032258064516129</v>
       </c>
-      <c r="K16" t="n">
+      <c r="L16" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="inlineStr">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
         <is>
           <t>Mean</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
-      <c r="F17" t="n">
-        <v>1</v>
-      </c>
+      <c r="F17" t="inlineStr"/>
       <c r="G17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H17" t="n">
-        <v>0.8282352941176473</v>
+        <v>0</v>
       </c>
       <c r="I17" t="n">
         <v>0.8282352941176473</v>
       </c>
       <c r="J17" t="n">
+        <v>0.8282352941176473</v>
+      </c>
+      <c r="K17" t="n">
         <v>0.9046594982078855</v>
       </c>
-      <c r="K17" t="n">
+      <c r="L17" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3013,7 +3205,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K17"/>
+  <dimension ref="A1:L17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3022,148 +3214,154 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>species</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>tp</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>fp</t>
         </is>
       </c>
-      <c r="D1" s="1" t="inlineStr">
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>fn</t>
         </is>
       </c>
-      <c r="E1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>tn</t>
         </is>
       </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="G1" s="1" t="inlineStr">
         <is>
           <t>sens</t>
         </is>
       </c>
-      <c r="G1" s="1" t="inlineStr">
+      <c r="H1" s="1" t="inlineStr">
         <is>
           <t>spec</t>
         </is>
       </c>
-      <c r="H1" s="1" t="inlineStr">
+      <c r="I1" s="1" t="inlineStr">
         <is>
           <t>prec</t>
         </is>
       </c>
-      <c r="I1" s="1" t="inlineStr">
+      <c r="J1" s="1" t="inlineStr">
         <is>
           <t>acc</t>
         </is>
       </c>
-      <c r="J1" s="1" t="inlineStr">
+      <c r="K1" s="1" t="inlineStr">
         <is>
           <t>f1</t>
         </is>
       </c>
-      <c r="K1" s="1" t="inlineStr">
+      <c r="L1" s="1" t="inlineStr">
         <is>
           <t>Threshold</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="B2" t="inlineStr">
         <is>
           <t>ACHROMOBACTER_XYLOSOXIDANS</t>
         </is>
       </c>
-      <c r="B2" t="n">
-        <v>4</v>
-      </c>
       <c r="C2" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" t="n">
         <v>0</v>
       </c>
       <c r="F2" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H2" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="I2" t="n">
         <v>0.8</v>
       </c>
       <c r="J2" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K2" t="n">
         <v>0.888888888888889</v>
       </c>
-      <c r="K2" t="n">
+      <c r="L2" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="1" t="inlineStr">
+      <c r="A3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="B3" t="inlineStr">
         <is>
           <t>ACINETOBACTER_BAUMANNII</t>
         </is>
       </c>
-      <c r="B3" t="n">
-        <v>4</v>
-      </c>
       <c r="C3" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3" t="n">
         <v>0</v>
       </c>
       <c r="F3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H3" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="I3" t="n">
         <v>0.8</v>
       </c>
       <c r="J3" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K3" t="n">
         <v>0.888888888888889</v>
       </c>
-      <c r="K3" t="n">
+      <c r="L3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="1" t="inlineStr">
+      <c r="A4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>AEROMONAS_HYDROPHILA</t>
         </is>
       </c>
-      <c r="B4" t="n">
+      <c r="C4" t="n">
         <v>5</v>
       </c>
-      <c r="C4" t="n">
-        <v>0</v>
-      </c>
       <c r="D4" t="n">
         <v>0</v>
       </c>
@@ -3171,12 +3369,12 @@
         <v>0</v>
       </c>
       <c r="F4" t="n">
-        <v>1</v>
-      </c>
-      <c r="G4" t="inlineStr"/>
-      <c r="H4" t="n">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G4" t="n">
+        <v>1</v>
+      </c>
+      <c r="H4" t="inlineStr"/>
       <c r="I4" t="n">
         <v>1</v>
       </c>
@@ -3184,132 +3382,144 @@
         <v>1</v>
       </c>
       <c r="K4" t="n">
+        <v>1</v>
+      </c>
+      <c r="L4" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="1" t="inlineStr">
+      <c r="A5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>ENTEROCOCCUS_FAECALIS</t>
         </is>
       </c>
-      <c r="B5" t="n">
-        <v>4</v>
-      </c>
       <c r="C5" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" t="n">
         <v>0</v>
       </c>
       <c r="F5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="I5" t="n">
         <v>0.8</v>
       </c>
       <c r="J5" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K5" t="n">
         <v>0.888888888888889</v>
       </c>
-      <c r="K5" t="n">
+      <c r="L5" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="1" t="inlineStr">
+      <c r="A6" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>ESCHERICHIA_COLI</t>
         </is>
       </c>
-      <c r="B6" t="n">
-        <v>4</v>
-      </c>
       <c r="C6" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
       </c>
       <c r="F6" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H6" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="I6" t="n">
         <v>0.8</v>
       </c>
       <c r="J6" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K6" t="n">
         <v>0.888888888888889</v>
       </c>
-      <c r="K6" t="n">
+      <c r="L6" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="1" t="inlineStr">
+      <c r="A7" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>KLEBSIELLA_PNEUMONIAE</t>
         </is>
       </c>
-      <c r="B7" t="n">
-        <v>4</v>
-      </c>
       <c r="C7" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E7" t="n">
         <v>0</v>
       </c>
       <c r="F7" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="I7" t="n">
         <v>0.8</v>
       </c>
       <c r="J7" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K7" t="n">
         <v>0.888888888888889</v>
       </c>
-      <c r="K7" t="n">
+      <c r="L7" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="1" t="inlineStr">
+      <c r="A8" s="1" t="n">
+        <v>6</v>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>LEGIONELLA_PNEUMOPHILA</t>
         </is>
       </c>
-      <c r="B8" t="n">
+      <c r="C8" t="n">
         <v>5</v>
       </c>
-      <c r="C8" t="n">
-        <v>0</v>
-      </c>
       <c r="D8" t="n">
         <v>0</v>
       </c>
@@ -3317,12 +3527,12 @@
         <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>1</v>
-      </c>
-      <c r="G8" t="inlineStr"/>
-      <c r="H8" t="n">
-        <v>1</v>
-      </c>
+        <v>0</v>
+      </c>
+      <c r="G8" t="n">
+        <v>1</v>
+      </c>
+      <c r="H8" t="inlineStr"/>
       <c r="I8" t="n">
         <v>1</v>
       </c>
@@ -3330,315 +3540,345 @@
         <v>1</v>
       </c>
       <c r="K8" t="n">
+        <v>1</v>
+      </c>
+      <c r="L8" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="1" t="inlineStr">
+      <c r="A9" s="1" t="n">
+        <v>7</v>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>LISTERIA_MONOCYTOGENES</t>
         </is>
       </c>
-      <c r="B9" t="n">
-        <v>4</v>
-      </c>
       <c r="C9" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E9" t="n">
         <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H9" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="I9" t="n">
         <v>0.8</v>
       </c>
       <c r="J9" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K9" t="n">
         <v>0.888888888888889</v>
       </c>
-      <c r="K9" t="n">
+      <c r="L9" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="1" t="inlineStr">
+      <c r="A10" s="1" t="n">
+        <v>8</v>
+      </c>
+      <c r="B10" t="inlineStr">
         <is>
           <t>NEISSERIA_MENINGITIDIS</t>
         </is>
       </c>
-      <c r="B10" t="n">
-        <v>4</v>
-      </c>
       <c r="C10" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E10" t="n">
         <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H10" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="I10" t="n">
         <v>0.8</v>
       </c>
       <c r="J10" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K10" t="n">
         <v>0.888888888888889</v>
       </c>
-      <c r="K10" t="n">
+      <c r="L10" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="1" t="inlineStr">
+      <c r="A11" s="1" t="n">
+        <v>9</v>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>SALMONELLA_ENTERICA</t>
         </is>
       </c>
-      <c r="B11" t="n">
-        <v>4</v>
-      </c>
       <c r="C11" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E11" t="n">
         <v>0</v>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="I11" t="n">
         <v>0.8</v>
       </c>
       <c r="J11" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K11" t="n">
         <v>0.888888888888889</v>
       </c>
-      <c r="K11" t="n">
+      <c r="L11" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="1" t="inlineStr">
+      <c r="A12" s="1" t="n">
+        <v>10</v>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>SHIGELLA_SONNEI</t>
         </is>
       </c>
-      <c r="B12" t="n">
-        <v>0</v>
-      </c>
       <c r="C12" t="n">
         <v>0</v>
       </c>
       <c r="D12" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E12" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F12" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G12" t="n">
-        <v>1</v>
-      </c>
-      <c r="H12" t="inlineStr"/>
-      <c r="I12" t="n">
+        <v>0</v>
+      </c>
+      <c r="H12" t="n">
+        <v>1</v>
+      </c>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="n">
         <v>0.2</v>
       </c>
-      <c r="J12" t="inlineStr"/>
-      <c r="K12" t="n">
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="1" t="inlineStr">
+      <c r="A13" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B13" t="inlineStr">
         <is>
           <t>STAPHYLOCOCCUS_AUREUS</t>
         </is>
       </c>
-      <c r="B13" t="n">
-        <v>4</v>
-      </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E13" t="n">
         <v>0</v>
       </c>
       <c r="F13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H13" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="I13" t="n">
         <v>0.8</v>
       </c>
       <c r="J13" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K13" t="n">
         <v>0.888888888888889</v>
       </c>
-      <c r="K13" t="n">
+      <c r="L13" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="1" t="inlineStr">
+      <c r="A14" s="1" t="n">
+        <v>12</v>
+      </c>
+      <c r="B14" t="inlineStr">
         <is>
           <t>STREPTOCOCCUS_PYOGENES</t>
         </is>
       </c>
-      <c r="B14" t="n">
-        <v>4</v>
-      </c>
       <c r="C14" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E14" t="n">
         <v>0</v>
       </c>
       <c r="F14" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H14" t="n">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="I14" t="n">
         <v>0.8</v>
       </c>
       <c r="J14" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="K14" t="n">
         <v>0.888888888888889</v>
       </c>
-      <c r="K14" t="n">
+      <c r="L14" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="1" t="inlineStr">
+      <c r="A15" s="1" t="n">
+        <v>13</v>
+      </c>
+      <c r="B15" t="inlineStr">
         <is>
           <t>VIBRIO_FURNISSII</t>
         </is>
       </c>
-      <c r="B15" t="n">
-        <v>0</v>
-      </c>
       <c r="C15" t="n">
         <v>0</v>
       </c>
       <c r="D15" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E15" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="F15" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G15" t="n">
-        <v>1</v>
-      </c>
-      <c r="H15" t="inlineStr"/>
-      <c r="I15" t="n">
+        <v>0</v>
+      </c>
+      <c r="H15" t="n">
+        <v>1</v>
+      </c>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="n">
         <v>0.2</v>
       </c>
-      <c r="J15" t="inlineStr"/>
-      <c r="K15" t="n">
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="1" t="inlineStr">
+      <c r="A16" s="1" t="n">
+        <v>14</v>
+      </c>
+      <c r="B16" t="inlineStr">
         <is>
           <t>Harmonic Mean</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr"/>
       <c r="E16" t="inlineStr"/>
-      <c r="F16" t="n">
-        <v>0</v>
-      </c>
+      <c r="F16" t="inlineStr"/>
       <c r="G16" t="n">
         <v>0</v>
       </c>
       <c r="H16" t="n">
+        <v>0</v>
+      </c>
+      <c r="I16" t="n">
         <v>0.8275862068965517</v>
       </c>
-      <c r="I16" t="n">
+      <c r="J16" t="n">
         <v>0.5714285714285714</v>
       </c>
-      <c r="J16" t="n">
+      <c r="K16" t="n">
         <v>0.9056603773584906</v>
       </c>
-      <c r="K16" t="n">
+      <c r="L16" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="1" t="inlineStr">
+      <c r="A17" s="1" t="n">
+        <v>15</v>
+      </c>
+      <c r="B17" t="inlineStr">
         <is>
           <t>Mean</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr"/>
       <c r="E17" t="inlineStr"/>
-      <c r="F17" t="n">
-        <v>0.8</v>
-      </c>
+      <c r="F17" t="inlineStr"/>
       <c r="G17" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="H17" t="n">
         <v>0.1538461538461539</v>
       </c>
-      <c r="H17" t="n">
+      <c r="I17" t="n">
         <v>0.8328912466843502</v>
       </c>
-      <c r="I17" t="n">
+      <c r="J17" t="n">
         <v>0.7314285714285714</v>
       </c>
-      <c r="J17" t="n">
+      <c r="K17" t="n">
         <v>0.9072730204805678</v>
       </c>
-      <c r="K17" t="n">
+      <c r="L17" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed capitalization in confusion mtx
</commit_message>
<xml_diff>
--- a/python_src/nist_confusion/confusion_matrix_0.0.xlsx
+++ b/python_src/nist_confusion/confusion_matrix_0.0.xlsx
@@ -1066,13 +1066,13 @@
         <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>0.9811320754716981</v>
+        <v>0.9811320754716982</v>
       </c>
       <c r="J16" t="n">
         <v>0.6746987951807228</v>
       </c>
       <c r="K16" t="n">
-        <v>0.8813559322033899</v>
+        <v>0.8813559322033898</v>
       </c>
       <c r="L16" t="n">
         <v>0</v>
@@ -2448,13 +2448,13 @@
       <c r="E16" t="inlineStr"/>
       <c r="F16" t="inlineStr"/>
       <c r="G16" t="n">
-        <v>0.8275862068965517</v>
+        <v>0.8275862068965516</v>
       </c>
       <c r="H16" t="n">
         <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>0.9655172413793104</v>
+        <v>0.9655172413793103</v>
       </c>
       <c r="J16" t="n">
         <v>0.835820895522388</v>
@@ -3150,10 +3150,10 @@
         <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>0.8235294117647058</v>
+        <v>0.823529411764706</v>
       </c>
       <c r="J16" t="n">
-        <v>0.8235294117647058</v>
+        <v>0.823529411764706</v>
       </c>
       <c r="K16" t="n">
         <v>0.9032258064516129</v>
@@ -3838,13 +3838,13 @@
         <v>0</v>
       </c>
       <c r="I16" t="n">
-        <v>0.8275862068965517</v>
+        <v>0.8275862068965518</v>
       </c>
       <c r="J16" t="n">
         <v>0.5714285714285714</v>
       </c>
       <c r="K16" t="n">
-        <v>0.9056603773584906</v>
+        <v>0.9056603773584905</v>
       </c>
       <c r="L16" t="n">
         <v>0</v>

</xml_diff>